<commit_message>
template files are modified
</commit_message>
<xml_diff>
--- a/templates/cpr1000/cin_check_list.xlsx
+++ b/templates/cpr1000/cin_check_list.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/churui/Projects/doc-server/templates/cpr1000/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\docServer\templates\cpr1000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="3680" windowWidth="27240" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="600" yWindow="3675" windowWidth="27240" windowHeight="14895" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <r>
       <t xml:space="preserve">安全级DCS </t>
@@ -43,24 +43,6 @@
     </r>
   </si>
   <si>
-    <t>项目名称</t>
-  </si>
-  <si>
-    <t>文件名称</t>
-  </si>
-  <si>
-    <t>检查</t>
-  </si>
-  <si>
-    <t>确认</t>
-  </si>
-  <si>
-    <t>文件版本</t>
-  </si>
-  <si>
-    <t>日期</t>
-  </si>
-  <si>
     <t>分类</t>
   </si>
   <si>
@@ -220,13 +202,95 @@
   <si>
     <t>${project} ${n_o_t} ${site_stage} site modification of ${cabinet}</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${r}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>项目名称</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件名称</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>检查</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>确认</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文件版本</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>日期</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,14 +338,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -314,6 +370,26 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -613,35 +689,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -674,18 +735,105 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -695,71 +843,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -775,6 +863,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1043,394 +1134,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
+    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:10" ht="60" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="32"/>
+    </row>
+    <row r="2" spans="1:10" ht="36" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="24.75" customHeight="1">
+      <c r="A3" s="34"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="40"/>
+      <c r="G3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="33" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="2" t="s">
+      <c r="C4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="4" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="18" customHeight="1">
+      <c r="A5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="47" t="s">
+      <c r="D5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="7" t="s">
+      <c r="E5" s="46"/>
+      <c r="F5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1">
+      <c r="A6" s="41"/>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="32" t="s">
+      <c r="C6" s="43"/>
+      <c r="D6" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="E6" s="49"/>
+      <c r="F6" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1">
+      <c r="A7" s="41"/>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="C7" s="44"/>
+      <c r="D7" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="25" t="s">
+      <c r="E7" s="46"/>
+      <c r="F7" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="32"/>
-      <c r="B6" s="9" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" customHeight="1">
+      <c r="A8" s="41"/>
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="26" t="s">
+      <c r="C8" s="42"/>
+      <c r="D8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="25" t="s">
+      <c r="E8" s="49"/>
+      <c r="F8" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="32"/>
-      <c r="B7" s="9" t="s">
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1">
+      <c r="A9" s="41"/>
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="33" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="33" t="s">
+      <c r="E9" s="49"/>
+      <c r="F9" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="32"/>
-      <c r="B8" s="9" t="s">
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="18" customHeight="1">
+      <c r="A10" s="41"/>
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="26" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="25" t="s">
+      <c r="E10" s="49"/>
+      <c r="F10" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="32"/>
-      <c r="B9" s="9" t="s">
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" customHeight="1">
+      <c r="A11" s="41"/>
+      <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="26" t="s">
+      <c r="C11" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="25" t="s">
+      <c r="D11" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="32"/>
-      <c r="B10" s="9" t="s">
+      <c r="E11" s="49"/>
+      <c r="F11" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="26" t="s">
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="18" customHeight="1">
+      <c r="A12" s="41"/>
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="25" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="32"/>
-      <c r="B11" s="9" t="s">
+      <c r="E12" s="49"/>
+      <c r="F12" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="18" customHeight="1">
+      <c r="A13" s="41"/>
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="25" t="s">
+      <c r="E13" s="49"/>
+      <c r="F13" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="32"/>
-      <c r="B12" s="9" t="s">
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="18" customHeight="1">
+      <c r="A14" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="26" t="s">
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="25" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="32"/>
-      <c r="B13" s="9" t="s">
+      <c r="E14" s="49"/>
+      <c r="F14" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="26" t="s">
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="18" customHeight="1">
+      <c r="A15" s="51"/>
+      <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="25" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="28" t="s">
+      <c r="E15" s="49"/>
+      <c r="F15" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="18" customHeight="1">
+      <c r="A16" s="51"/>
+      <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="26" t="s">
+      <c r="E16" s="49"/>
+      <c r="F16" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" ht="18" customHeight="1">
+      <c r="A17" s="51"/>
+      <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="25" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="28"/>
-      <c r="B15" s="9" t="s">
+      <c r="E17" s="49"/>
+      <c r="F17" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" ht="31.5" customHeight="1" thickBot="1">
+      <c r="A19" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="28"/>
-      <c r="B16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="28"/>
-      <c r="B17" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18"/>
-    </row>
-    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="24"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:H13"/>
@@ -1447,9 +1529,31 @@
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>